<commit_message>
Finalize Malayalam batch pipeline and sync media counts
</commit_message>
<xml_diff>
--- a/109 Languages Frequency Word Lists/Malayalam (ML).xlsx
+++ b/109 Languages Frequency Word Lists/Malayalam (ML).xlsx
@@ -468,7 +468,7 @@
         <v>10</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3">
@@ -481,10 +481,10 @@
         <v>10</v>
       </c>
       <c r="C3" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D3" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4">
@@ -497,10 +497,10 @@
         <v>10</v>
       </c>
       <c r="C4" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D4" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5">

</xml_diff>